<commit_message>
Apply new theme for splash screen Added search question functionality Added increase/decrease font menu
</commit_message>
<xml_diff>
--- a/DB/DB_JIQ.xlsx
+++ b/DB/DB_JIQ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="442">
   <si>
     <t>ID</t>
   </si>
@@ -1250,17 +1250,6 @@
 .</t>
   </si>
   <si>
-    <t>Ans)
-Differences between threads and processes are:-
-1. Threads share the address space of the process that &amp;nbsp;created it; processes have their own address.
-2. Threads have direct access to the data segment of its process;  processes have their own copy of the data segment of the parent process.
-3. Threads can directly communicate with other threads of its  process; processes must use interprocess communication to communicate with  sibling processes.
-4. Threads have almost no overhead; processes have considerable  overhead.
-5. New threads are easily created; new processes require duplication  of the parent process.
-6. Threads can exercise considerable control over threads of  the same process; processes can only exercise control over child processes.
-7. Changes to the main thread (cancellation, priority change,  etc.) may affect the behavior of the other threads of the process; changes to  the parent process do not affect child processes.</t>
-  </si>
-  <si>
     <t>What are the two ways of creating thread?</t>
   </si>
   <si>
@@ -1317,21 +1306,6 @@
 A thread of execution.
 An instance of Thread is just&amp;hellip;an object. Like any other object in Java, it has variables and methods, and lives and dies on the heap. But a thread of execution is an individual process (a "lightweight" process) that has its own call stack. In Java, there is one thread per call stack&amp;mdash;or, to think of it in reverse, one call stack per thread. Even if you don""t create any new threads in your program, threads are back there running.
 The main() method, that starts the whole ball rolling, runs in one thread, called (surprisingly) the main thread. If you looked at the main call stack (and you can, any time you get a stack trace from something that happens after main begins, but not within another thread), you""d see that main() is the first method on the stack&amp;mdash; the method at the bottom. But as soon as you create a new thread, a new stack materializes and methods called from that thread run in a call stack that""s separate from the main() call stack.</t>
-  </si>
-  <si>
-    <t>Ans)
-&amp;nbsp;
-Threads support  concurrent operations. For example,
-&amp;nbsp;&amp;bull; Multiple requests by a client on  a server can be handled as an individual client thread.
-&amp;nbsp;&amp;bull; Long computations or high-latency  disk and network operations can be handled in the background without disturbing  foreground computations or screen updates.
-Threads often result in simpler programs.
-&amp;bull; In sequential programming,  updating multiple displays normally requires a big while-loop that performs  small parts of each display update. Unfortunately, this loop basically  simulates an operating system scheduler. In Java, each view can be assigned a  thread to provide continuous updates.
-&amp;bull; Programs that need to respond to  user-initiated events can set up service routines to handle the events without  having to insert code in the main routine to look for these events.
-Threads provide a high degree of control.
-&amp;bull; Imagine launching a complex  computation that occasionally takes longer than is satisfactory. A  "watchdog" thread can be activated that will "kill" the computation  if it becomes costly, perhaps in favor of an alternate, approximate solution. Note  that sequential programs must muddy the computation with termination code,  whereas, a Java program can use thread control to non-intrusively supervise any  operation.
-Threaded applications exploit parallelism.
-&amp;bull; A computer with multiple CPUs can  literally execute multiple threads on different functional units without having  to simulating multi-tasking ("time sharing").
-&amp;bull; On some computers, one CPU  handles the display while another handles computations or database accesses,  thus, providing extremely fast user interface response times.</t>
   </si>
   <si>
     <t>Ans) There are two ways to create a new thread.
@@ -1372,9 +1346,6 @@
             synchronized (this){             // synchronized keyword on block of  code
             }
 }</t>
-  </si>
-  <si>
-    <t>Ans) When a synch non static method is called a lock is obtained on the object. When a synch static method is called a lock is obtained on the class and not on the object. The lock on the object and the lock on the class donâ€™t interfere with each other. It means, a thread accessing a synch non static method, then the other thread can access the synch static method at the same time but canâ€™t access the synch non static method.</t>
   </si>
   <si>
     <t>Ans) In general each thread has its own copy of variable, such that one thread is not concerned with the value of same variable in the other thread. But sometime this may not be the case. Consider a scenario in which the count variable is holding the number of times a method is called for a given class irrespective of any thread calling, in this case irrespective of thread access the count has to be increased so the count variable is declared as volatile. The copy of volatile variable is stored in the main memory, so every time a thread access the variable even for reading purpose the local copy is updated each time from the main memory. The volatile variable also have performance issues.</t>
@@ -2280,67 +2251,6 @@
 Immutable class is a class which once created, it&amp;rsquo;s contents can  not be changed.
 Immutable objects are the objects whose  state can not be changed once constructed.
 e.g. String class</t>
-  </si>
-  <si>
-    <t>Ans)
-To create an immutable class following steps should be followed:
-Create a final class.
-Set the values of properties  using constructor only.
-Make the properties of the  class final and private
-Do not provide any setters for  these properties.
-If the instance fields include  references to mutable objects, don''t allow those objects to be changed:
-Don''t provide methods that  modify the mutable objects.
-Don''t share references to the  mutable objects. Never store references to external, mutable objects passed to  the constructor; if necessary, create copies, and store references to the  copies. Similarly, create copies of your internal mutable objects when  necessary to avoid returning the originals in your methods.
-E.g.
-public
-final
-class
-FinalPersonClass {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-private
-final
-String name;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-private
-final
-int
-age;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-public
-FinalPersonClass(
-final
-String name,
-final
-int
-age) {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-super
-();
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-this
-.name = name;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-this
-.age = age;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; }
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-public
-int
-getAge() {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-return
-age;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; }
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-public
-String getName() {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-return
-name;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; }
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-}</t>
   </si>
   <si>
     <t>Ans)
@@ -2721,6 +2631,247 @@
   </si>
   <si>
     <t>What are the advantages or usage of threads?</t>
+  </si>
+  <si>
+    <t>Ans)
+Differences between threads and processes are:-
+1. Threads share the address space of the process that  created it; processes have their own address.
+2. Threads have direct access to the data segment of its process;  processes have their own copy of the data segment of the parent process.
+3. Threads can directly communicate with other threads of its  process; processes must use interprocess communication to communicate with  sibling processes.
+4. Threads have almost no overhead; processes have considerable  overhead.
+5. New threads are easily created; new processes require duplication  of the parent process.
+6. Threads can exercise considerable control over threads of  the same process; processes can only exercise control over child processes.
+7. Changes to the main thread (cancellation, priority change,  etc.) may affect the behavior of the other threads of the process; changes to  the parent process do not affect child processes.</t>
+  </si>
+  <si>
+    <t>Ans)
+To create an immutable class following steps should be followed:
+Create a final class.
+Set the values of properties  using constructor only.
+Make the properties of the  class final and private
+Do not provide any setters for  these properties.
+If the instance fields include  references to mutable objects, don''t allow those objects to be changed:
+Don''t provide methods that  modify the mutable objects.
+Don''t share references to the  mutable objects. Never store references to external, mutable objects passed to  the constructor; if necessary, create copies, and store references to the  copies. Similarly, create copies of your internal mutable objects when  necessary to avoid returning the originals in your methods.
+E.g.
+public
+final
+class
+FinalPersonClass {
+private
+final
+String name;
+private
+final
+int
+age;
+public
+FinalPersonClass(
+final
+String name,
+final
+int
+age) {
+super
+();
+this
+.name = name;
+this
+.age = age;
+      }
+public
+int
+getAge() {
+return
+age;
+      }
+public
+String getName() {
+return
+name;
+      }
+}</t>
+  </si>
+  <si>
+    <t>Ans)
+Threads support  concurrent operations. For example,
+ - Multiple requests by a client on  a server can be handled as an individual client thread.
+ - Long computations or high-latency  disk and network operations can be handled in the background without disturbing  foreground computations or screen updates.
+Threads often result in simpler programs.
+- In sequential programming,  updating multiple displays normally requires a big while-loop that performs  small parts of each display update. Unfortunately, this loop basically  simulates an operating system scheduler. In Java, each view can be assigned a  thread to provide continuous updates.
+- Programs that need to respond to  user-initiated events can set up service routines to handle the events without  having to insert code in the main routine to look for these events.
+Threads provide a high degree of control.
+- Imagine launching a complex  computation that occasionally takes longer than is satisfactory. A  "watchdog" thread can be activated that will "kill" the computation  if it becomes costly, perhaps in favor of an alternate, approximate solution. Note  that sequential programs must muddy the computation with termination code,  whereas, a Java program can use thread control to non-intrusively supervise any  operation.
+Threaded applications exploit parallelism.
+- A computer with multiple CPUs can  literally execute multiple threads on different functional units without having  to simulating multi-tasking ("time sharing").
+- On some computers, one CPU  handles the display while another handles computations or database accesses,  thus, providing extremely fast user interface response times.</t>
+  </si>
+  <si>
+    <t>Ans) When a synch non static method is called a lock is obtained on the object. When a synch static method is called a lock is obtained on the class and not on the object. The lock on the object and the lock on the class don''t interfere with each other. It means, a thread accessing a synch non static method, then the other thread can access the synch static method at the same time but can''t access the synch non static method.</t>
+  </si>
+  <si>
+    <t>Does java support multiple interitance? Why?</t>
+  </si>
+  <si>
+    <t>Ans) Java doesnt support multiple inheritance but it provide a way through which it can enact it. 
+Consider the scenario is C++
+Class A{
+public void add(){
+// some text
+}
+}
+Class B{
+public void add(){
+// some text
+}
+}
+Class C extends A,B{
+public static void main(String arg[]){
+C objC = new C();
+objC.add(); // problem, compiler gets confused and cant
+decide to call Class A or B method.
+}
+This problem is called Diamond problem.
+This problem in java is taken care with the use of interfaces
+In Java similar problem would look like:
+interface A{
+add();
+}
+interface B{
+add();
+}
+class C implements A,B{
+add(){
+// doesnt matter which interface it belong to
+}
+}</t>
+  </si>
+  <si>
+    <t>Can this keyword be assigned null value?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>What are the different types of references in java?</t>
+  </si>
+  <si>
+    <t>Ans) Java has a more expressive system of reference than most other garbage-collected programming languages, which allows for special behavior for garbage collection. A normal reference in Java is known as a strong reference. The java.lang.ref package defines three other types of references—soft, weak, and phantom references. Each type of reference is designed for a specific use.
+A SoftReference can be used to implement a cache. An object that is not reachable by a strong reference (that is, not strongly reachable), but is referenced by a soft reference is called softly reachable. A softly reachable object may be garbage collected at the discretion of the garbage collector. This generally means that softly reachable objects will only be garbage collected when free memory is low, but again, it is at the discretion of the garbage collector. Semantically, a soft reference means "keep this object unless the memory is needed."
+A WeakReference is used to implement weak maps. An object that is not strongly or softly reachable, but is referenced by a weak reference is called weakly reachable. A weakly reachable object will be garbage collected during the next collection cycle. This behavior is used in the class java.util.WeakHashMap. A weak map allows the programmer to put key/value pairs in the map and not worry about the objects taking up memory when the key is no longer reachable anywhere else. Another possible application of weak references is the string intern pool. Semantically, a weak reference means "get rid of this object when nothing else references it."
+A PhantomReference is used to reference objects that have been marked for garbage collection and have been finalized, but have not yet been reclaimed. An object that is not strongly, softly or weakly reachable, but is referenced by a phantom reference is called phantom reachable. This allows for more flexible cleanup than is possible with the finalization mechanism alone. Semantically, a phantom reference means "this object is no longer needed and has been finalized in preparation for being collected."</t>
+  </si>
+  <si>
+    <t>How to change the heap size of a JVM?</t>
+  </si>
+  <si>
+    <t>What is difference between instanceof and isInstance(Object obj)?</t>
+  </si>
+  <si>
+    <t>Ans) Differences are as follows:
+1) instanceof is a reserved word of Java, but isInstance(Object obj) is a method of java.lang.Class.
+if (obj instanceof MyType) {
+...
+}else if (MyType.class.isInstance(obj)) {
+...
+}
+2) instanceof is used of identify whether the object is type of a particular class or its subclass but isInstance(obj) is used to identify object of a particular class.</t>
+  </si>
+  <si>
+    <t>Java supports pass by value or pass by reference?</t>
+  </si>
+  <si>
+    <t>Ans) Java supports only pass by value. The arguments passed as a parameter to a method is mainly primitive data types or objects. For the data type the actual value is passed.
+Java passes the references by value just like any other parameter. This means the references passed to the method are actually copies of the original references.Java copies and passes the reference by value, not the object. Thus, method manipulation will alter the objects, since the references point to the original objects.Consider the example:
+ public void tricky(Point arg1, Point arg2)
+ {
+   arg1.x = 100;
+   arg1.y = 100;
+   Point temp = arg1;
+   arg1 = arg2;
+   arg2 = temp;
+ }
+ public static void main(String [] args)
+ {
+   Point pnt1 = new Point(0,0);
+   Point pnt2 = new Point(0,0);
+   System.out.println("X: " + pnt1.x + " Y: " +pnt1.y); 
+   System.out.println("X: " + pnt2.x + " Y: " +pnt2.y);
+   System.out.println(" ");
+   tricky(pnt1,pnt2);
+   System.out.println("X: " + pnt1.x + " Y:" + pnt1.y); 
+   System.out.println("X: " + pnt2.x + " Y: " +pnt2.y); 
+ }
+OutPut:
+X: 0 Y: 0
+X: 0 Y: 0
+X: 100 Y: 100
+X: 0 Y: 0
+The method successfully alters the value of pnt1, even though it is passed by value; however, a swap of pnt1 and pnt2 fails! This is the major source of confusion. In the main() method, pnt1 and pnt2 are nothing more than object references. When you pass pnt1 and pnt2 to the tricky() method, Java passes the references by value just like any other parameter. This means the references passed to the method are actually copies of the original references.</t>
+  </si>
+  <si>
+    <t>What is memory leak?</t>
+  </si>
+  <si>
+    <t>Ans) A memory leak is where an unreferenced object that will never be used again still hangs around in memory and doesnt get garbage collected.</t>
+  </si>
+  <si>
+    <t>What is the difference between equals() and ==?</t>
+  </si>
+  <si>
+    <t>Ans) == operator is used to compare the references of the objects. 
+public bollean equals(Object o) is the method provided by the Object class. The default implementation uses == operator to compare two objects.
+But since the method can be overriden like for String class. equals() method can be used to compare the values of two objects.
+ String str1 = "MyName"; 
+ String str2 = "MyName";
+ String str3 = str2;
+ if(str1 == str2){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ if(str1.equals(str2)){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ Output:
+ Objects are not equal
+ Objects are equal
+ String str2 = "MyName";
+ String str3 = str2;
+ if(str2 == str3){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ if(str3.equals(str2)){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ OutPut:
+ Objects are equal
+ Objects are equal</t>
+  </si>
+  <si>
+    <t>How to make sure that Childclass method actually overrides the method of the superclass?</t>
+  </si>
+  <si>
+    <t>Ans) The @Override annotation can be added to the javadoc for the new method. If you accidently miss an argument or capitalize the method name wrong, the compiler will generate a compile-time error.</t>
+  </si>
+  <si>
+    <t>How to find the size of an object?</t>
+  </si>
+  <si>
+    <t>Ans)The heap size of an object can be found using -
+         Runtime.totalMemory()-Runtime.freeMemory() .</t>
+  </si>
+  <si>
+    <t>Ans) The old generation''s default heap size can be overridden by using the -Xms and -Xmx switches to specify the initial and maximum sizes respectively: 
+java -Xms &lt;initial size&gt; -Xmx &lt;maximum size&gt; program
+For example: 
+java -Xms64m -Xmx128m program</t>
   </si>
 </sst>
 </file>
@@ -3071,7 +3222,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3401,7 +3554,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3423,7 +3576,7 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
@@ -5238,7 +5391,7 @@
         <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5256,7 +5409,7 @@
         <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -5274,7 +5427,7 @@
         <v>6</v>
       </c>
       <c r="C104" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -5292,7 +5445,7 @@
         <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -5310,7 +5463,7 @@
         <v>6</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -5328,7 +5481,7 @@
         <v>6</v>
       </c>
       <c r="C107" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -5346,7 +5499,7 @@
         <v>6</v>
       </c>
       <c r="C108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -5364,7 +5517,7 @@
         <v>6</v>
       </c>
       <c r="C109" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -5382,7 +5535,7 @@
         <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -5400,7 +5553,7 @@
         <v>6</v>
       </c>
       <c r="C111" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -5418,7 +5571,7 @@
         <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -5436,7 +5589,7 @@
         <v>6</v>
       </c>
       <c r="C113" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -5454,7 +5607,7 @@
         <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -5472,7 +5625,7 @@
         <v>6</v>
       </c>
       <c r="C115" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -5490,7 +5643,7 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -5508,7 +5661,7 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -5526,7 +5679,7 @@
         <v>6</v>
       </c>
       <c r="C118" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -5544,7 +5697,7 @@
         <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -5562,7 +5715,7 @@
         <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -5580,7 +5733,7 @@
         <v>6</v>
       </c>
       <c r="C121" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -5598,7 +5751,7 @@
         <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -5616,7 +5769,7 @@
         <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -5634,7 +5787,7 @@
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -5652,7 +5805,7 @@
         <v>6</v>
       </c>
       <c r="C125" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -5670,7 +5823,7 @@
         <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -5688,7 +5841,7 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -5706,7 +5859,7 @@
         <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -5724,7 +5877,7 @@
         <v>6</v>
       </c>
       <c r="C129" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -5742,7 +5895,7 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -5760,7 +5913,7 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -5778,7 +5931,7 @@
         <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -5796,7 +5949,7 @@
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -5814,7 +5967,7 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -5832,7 +5985,7 @@
         <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -5850,7 +6003,7 @@
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D136">
         <v>0</v>
@@ -5868,7 +6021,7 @@
         <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -5886,7 +6039,7 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -5904,7 +6057,7 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D139">
         <v>0</v>
@@ -5922,7 +6075,7 @@
         <v>7</v>
       </c>
       <c r="C140" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D140">
         <v>0</v>
@@ -5940,7 +6093,7 @@
         <v>7</v>
       </c>
       <c r="C141" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -5958,7 +6111,7 @@
         <v>7</v>
       </c>
       <c r="C142" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -5976,7 +6129,7 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -5994,7 +6147,7 @@
         <v>7</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D144">
         <v>0</v>
@@ -6012,7 +6165,7 @@
         <v>7</v>
       </c>
       <c r="C145" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D145">
         <v>0</v>
@@ -6030,7 +6183,7 @@
         <v>7</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D146">
         <v>0</v>
@@ -6048,7 +6201,7 @@
         <v>7</v>
       </c>
       <c r="C147" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D147">
         <v>0</v>
@@ -6066,7 +6219,7 @@
         <v>7</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D148">
         <v>0</v>
@@ -6084,7 +6237,7 @@
         <v>7</v>
       </c>
       <c r="C149" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D149">
         <v>0</v>
@@ -6102,7 +6255,7 @@
         <v>7</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -6121,7 +6274,7 @@
         <v>7</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D151">
         <v>0</v>
@@ -6140,7 +6293,7 @@
         <v>7</v>
       </c>
       <c r="C152" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -6158,7 +6311,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D153">
         <v>0</v>
@@ -6177,7 +6330,7 @@
         <v>7</v>
       </c>
       <c r="C154" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -6195,7 +6348,7 @@
         <v>7</v>
       </c>
       <c r="C155" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -6213,7 +6366,7 @@
         <v>7</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D156">
         <v>0</v>
@@ -6232,7 +6385,7 @@
         <v>7</v>
       </c>
       <c r="C157" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -6250,7 +6403,7 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -6268,7 +6421,7 @@
         <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -6286,7 +6439,7 @@
         <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -6304,7 +6457,7 @@
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -6322,7 +6475,7 @@
         <v>8</v>
       </c>
       <c r="C162" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D162">
         <v>0</v>
@@ -6340,7 +6493,7 @@
         <v>8</v>
       </c>
       <c r="C163" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -6358,7 +6511,7 @@
         <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D164">
         <v>0</v>
@@ -6376,7 +6529,7 @@
         <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D165">
         <v>0</v>
@@ -6394,7 +6547,7 @@
         <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D166">
         <v>0</v>
@@ -6412,7 +6565,7 @@
         <v>8</v>
       </c>
       <c r="C167" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -6448,7 +6601,7 @@
         <v>8</v>
       </c>
       <c r="C169" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -6466,7 +6619,7 @@
         <v>8</v>
       </c>
       <c r="C170" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -6484,7 +6637,7 @@
         <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -6502,7 +6655,7 @@
         <v>8</v>
       </c>
       <c r="C172" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -6520,7 +6673,7 @@
         <v>9</v>
       </c>
       <c r="C173" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -6538,7 +6691,7 @@
         <v>9</v>
       </c>
       <c r="C174" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -6556,7 +6709,7 @@
         <v>9</v>
       </c>
       <c r="C175" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -6574,7 +6727,7 @@
         <v>9</v>
       </c>
       <c r="C176" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -6592,7 +6745,7 @@
         <v>9</v>
       </c>
       <c r="C177" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -6610,7 +6763,7 @@
         <v>10</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -6628,7 +6781,7 @@
         <v>10</v>
       </c>
       <c r="C179" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -6646,7 +6799,7 @@
         <v>10</v>
       </c>
       <c r="C180" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -6664,7 +6817,7 @@
         <v>10</v>
       </c>
       <c r="C181" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -6682,7 +6835,7 @@
         <v>10</v>
       </c>
       <c r="C182" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -6700,7 +6853,7 @@
         <v>10</v>
       </c>
       <c r="C183" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -6718,7 +6871,7 @@
         <v>11</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -6737,7 +6890,7 @@
         <v>11</v>
       </c>
       <c r="C185" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -6755,7 +6908,7 @@
         <v>11</v>
       </c>
       <c r="C186" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -6773,7 +6926,7 @@
         <v>11</v>
       </c>
       <c r="C187" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -6791,7 +6944,7 @@
         <v>11</v>
       </c>
       <c r="C188" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -6809,7 +6962,7 @@
         <v>11</v>
       </c>
       <c r="C189" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -6827,7 +6980,7 @@
         <v>11</v>
       </c>
       <c r="C190" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -6845,7 +6998,7 @@
         <v>11</v>
       </c>
       <c r="C191" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D191">
         <v>0</v>
@@ -6863,7 +7016,7 @@
         <v>11</v>
       </c>
       <c r="C192" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -6881,7 +7034,7 @@
         <v>11</v>
       </c>
       <c r="C193" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D193">
         <v>0</v>
@@ -6899,7 +7052,7 @@
         <v>11</v>
       </c>
       <c r="C194" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -6917,7 +7070,7 @@
         <v>11</v>
       </c>
       <c r="C195" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -6935,13 +7088,13 @@
         <v>11</v>
       </c>
       <c r="C196" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D196">
         <v>0</v>
       </c>
       <c r="E196" t="str">
-        <f t="shared" ref="E196:E199" si="3">"insert into Questions values("&amp;A196&amp;","&amp;B196&amp;",'Q) "&amp;C196&amp;"',"&amp;D196&amp;");"</f>
+        <f t="shared" ref="E196:E209" si="3">"insert into Questions values("&amp;A196&amp;","&amp;B196&amp;",'Q) "&amp;C196&amp;"',"&amp;D196&amp;");"</f>
         <v>insert into Questions values(195,11,'Q) How do I prevent the output of my JSP or Servlet pages from being cached by the browser?',0);</v>
       </c>
     </row>
@@ -6953,7 +7106,7 @@
         <v>11</v>
       </c>
       <c r="C197" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -6971,7 +7124,7 @@
         <v>11</v>
       </c>
       <c r="C198" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -6989,7 +7142,7 @@
         <v>11</v>
       </c>
       <c r="C199" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -6997,6 +7150,186 @@
       <c r="E199" t="str">
         <f t="shared" si="3"/>
         <v>insert into Questions values(198,11,'Q) Why is it not a good practice to create HttpSessions in JSPs by default?',0);</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
+        <v>422</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(199,2,'Q) Does java support multiple interitance? Why?',0);</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
+        <v>424</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(200,2,'Q) Can this keyword be assigned null value?',0);</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
+        <v>426</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(201,2,'Q) What are the different types of references in java?',0);</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
+        <v>428</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(202,2,'Q) How to change the heap size of a JVM?',0);</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+      <c r="C204" t="s">
+        <v>429</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(203,2,'Q) What is difference between instanceof and isInstance(Object obj)?',0);</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205">
+        <v>2</v>
+      </c>
+      <c r="C205" t="s">
+        <v>431</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(204,2,'Q) Java supports pass by value or pass by reference?',0);</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206">
+        <v>2</v>
+      </c>
+      <c r="C206" t="s">
+        <v>433</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(205,2,'Q) What is memory leak?',0);</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207">
+        <v>2</v>
+      </c>
+      <c r="C207" t="s">
+        <v>435</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(206,2,'Q) What is the difference between equals() and ==?',0);</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208">
+        <v>2</v>
+      </c>
+      <c r="C208" t="s">
+        <v>437</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(207,2,'Q) How to make sure that Childclass method actually overrides the method of the superclass?',0);</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209">
+        <v>2</v>
+      </c>
+      <c r="C209" t="s">
+        <v>439</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Questions values(208,2,'Q) How to find the size of an object?',0);</v>
       </c>
     </row>
   </sheetData>
@@ -7006,9 +7339,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="E200" sqref="E200:E209"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9396,7 +9731,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -9410,7 +9745,7 @@
 The main() method, that starts the whole ball rolling, runs in one thread, called (surprisingly) the main thread. If you looked at the main call stack (and you can, any time you get a stack trace from something that happens after main begins, but not within another thread), you""d see that main() is the first method on the stack&amp;mdash; the method at the bottom. But as soon as you create a new thread, a new stack materializes and methods called from that thread run in a call stack that""s separate from the main() call stack.',1);</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="360" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9418,7 +9753,7 @@
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>226</v>
+        <v>418</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -9427,7 +9762,7 @@
         <f t="shared" si="1"/>
         <v>insert into Answers values(102,102,'Ans)
 Differences between threads and processes are:-
-1. Threads share the address space of the process that &amp;nbsp;created it; processes have their own address.
+1. Threads share the address space of the process that  created it; processes have their own address.
 2. Threads have direct access to the data segment of its process;  processes have their own copy of the data segment of the parent process.
 3. Threads can directly communicate with other threads of its  process; processes must use interprocess communication to communicate with  sibling processes.
 4. Threads have almost no overhead; processes have considerable  overhead.
@@ -9444,7 +9779,7 @@
         <v>103</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>245</v>
+        <v>420</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -9452,18 +9787,17 @@
       <c r="E104" t="str">
         <f t="shared" si="1"/>
         <v>insert into Answers values(103,103,'Ans)
-&amp;nbsp;
 Threads support  concurrent operations. For example,
-&amp;nbsp;&amp;bull; Multiple requests by a client on  a server can be handled as an individual client thread.
-&amp;nbsp;&amp;bull; Long computations or high-latency  disk and network operations can be handled in the background without disturbing  foreground computations or screen updates.
+ - Multiple requests by a client on  a server can be handled as an individual client thread.
+ - Long computations or high-latency  disk and network operations can be handled in the background without disturbing  foreground computations or screen updates.
 Threads often result in simpler programs.
-&amp;bull; In sequential programming,  updating multiple displays normally requires a big while-loop that performs  small parts of each display update. Unfortunately, this loop basically  simulates an operating system scheduler. In Java, each view can be assigned a  thread to provide continuous updates.
-&amp;bull; Programs that need to respond to  user-initiated events can set up service routines to handle the events without  having to insert code in the main routine to look for these events.
+- In sequential programming,  updating multiple displays normally requires a big while-loop that performs  small parts of each display update. Unfortunately, this loop basically  simulates an operating system scheduler. In Java, each view can be assigned a  thread to provide continuous updates.
+- Programs that need to respond to  user-initiated events can set up service routines to handle the events without  having to insert code in the main routine to look for these events.
 Threads provide a high degree of control.
-&amp;bull; Imagine launching a complex  computation that occasionally takes longer than is satisfactory. A  "watchdog" thread can be activated that will "kill" the computation  if it becomes costly, perhaps in favor of an alternate, approximate solution. Note  that sequential programs must muddy the computation with termination code,  whereas, a Java program can use thread control to non-intrusively supervise any  operation.
+- Imagine launching a complex  computation that occasionally takes longer than is satisfactory. A  "watchdog" thread can be activated that will "kill" the computation  if it becomes costly, perhaps in favor of an alternate, approximate solution. Note  that sequential programs must muddy the computation with termination code,  whereas, a Java program can use thread control to non-intrusively supervise any  operation.
 Threaded applications exploit parallelism.
-&amp;bull; A computer with multiple CPUs can  literally execute multiple threads on different functional units without having  to simulating multi-tasking ("time sharing").
-&amp;bull; On some computers, one CPU  handles the display while another handles computations or database accesses,  thus, providing extremely fast user interface response times.',1);</v>
+- A computer with multiple CPUs can  literally execute multiple threads on different functional units without having  to simulating multi-tasking ("time sharing").
+- On some computers, one CPU  handles the display while another handles computations or database accesses,  thus, providing extremely fast user interface response times.',1);</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
@@ -9474,7 +9808,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -9513,7 +9847,7 @@
         <v>105</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -9535,7 +9869,7 @@
         <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -9559,14 +9893,14 @@
         <v>107</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>249</v>
+        <v>421</v>
       </c>
       <c r="D108">
         <v>1</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="1"/>
-        <v>insert into Answers values(107,107,'Ans) When a synch non static method is called a lock is obtained on the object. When a synch static method is called a lock is obtained on the class and not on the object. The lock on the object and the lock on the class donâ€™t interfere with each other. It means, a thread accessing a synch non static method, then the other thread can access the synch static method at the same time but canâ€™t access the synch non static method.',1);</v>
+        <v>insert into Answers values(107,107,'Ans) When a synch non static method is called a lock is obtained on the object. When a synch static method is called a lock is obtained on the class and not on the object. The lock on the object and the lock on the class don''t interfere with each other. It means, a thread accessing a synch non static method, then the other thread can access the synch static method at the same time but can''t access the synch non static method.',1);</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="150" x14ac:dyDescent="0.25">
@@ -9577,7 +9911,7 @@
         <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -9595,7 +9929,7 @@
         <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -9614,7 +9948,7 @@
         <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -9634,7 +9968,7 @@
         <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D112">
         <v>1</v>
@@ -9654,7 +9988,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -9672,7 +10006,7 @@
         <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -9690,7 +10024,7 @@
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -9708,7 +10042,7 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -9726,7 +10060,7 @@
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -9746,7 +10080,7 @@
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D118">
         <v>1</v>
@@ -9767,7 +10101,7 @@
         <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D119">
         <v>1</v>
@@ -9785,7 +10119,7 @@
         <v>119</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -9803,7 +10137,7 @@
         <v>120</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D121">
         <v>1</v>
@@ -9821,7 +10155,7 @@
         <v>121</v>
       </c>
       <c r="C122" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -9839,7 +10173,7 @@
         <v>122</v>
       </c>
       <c r="C123" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -9857,7 +10191,7 @@
         <v>123</v>
       </c>
       <c r="C124" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D124">
         <v>1</v>
@@ -9875,7 +10209,7 @@
         <v>124</v>
       </c>
       <c r="C125" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D125">
         <v>1</v>
@@ -9893,7 +10227,7 @@
         <v>125</v>
       </c>
       <c r="C126" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D126">
         <v>1</v>
@@ -9911,7 +10245,7 @@
         <v>126</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -9930,7 +10264,7 @@
         <v>127</v>
       </c>
       <c r="C128" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -9948,7 +10282,7 @@
         <v>128</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -9968,7 +10302,7 @@
         <v>129</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -9987,13 +10321,13 @@
         <v>130</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D131">
         <v>1</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" ref="E131:E199" si="2">"insert into Answers values("&amp;A131&amp;","&amp;B131&amp;",'"&amp;C131&amp;"',"&amp;D131&amp;");"</f>
+        <f t="shared" ref="E131:E200" si="2">"insert into Answers values("&amp;A131&amp;","&amp;B131&amp;",'"&amp;C131&amp;"',"&amp;D131&amp;");"</f>
         <v>insert into Answers values(130,130,'Ans) If a class is made to extend the thread class to have a multithreaded application then this subclass of Thread can not extend any other class and the required application will have to be added to this class as it can not be inherited from any other class.
       If a class is made to implement Runnable interface, then the class can extend other class or implement other interface.',1);</v>
       </c>
@@ -10006,7 +10340,7 @@
         <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -10024,7 +10358,7 @@
         <v>132</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D133">
         <v>1</v>
@@ -10049,7 +10383,7 @@
         <v>133</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -10070,7 +10404,7 @@
         <v>134</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -10096,7 +10430,7 @@
         <v>135</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -10118,7 +10452,7 @@
         <v>136</v>
       </c>
       <c r="C137" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -10136,7 +10470,7 @@
         <v>137</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -10158,7 +10492,7 @@
         <v>138</v>
       </c>
       <c r="C139" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D139">
         <v>1</v>
@@ -10176,7 +10510,7 @@
         <v>139</v>
       </c>
       <c r="C140" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -10194,7 +10528,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -10217,7 +10551,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D142">
         <v>1</v>
@@ -10250,7 +10584,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -10321,7 +10655,7 @@
         <v>143</v>
       </c>
       <c r="C144" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D144">
         <v>1</v>
@@ -10339,7 +10673,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -10390,7 +10724,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D146">
         <v>1</v>
@@ -10418,7 +10752,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D147">
         <v>1</v>
@@ -10501,7 +10835,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -10534,7 +10868,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D149">
         <v>1</v>
@@ -10568,7 +10902,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D150">
         <v>1</v>
@@ -10600,7 +10934,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D151">
         <v>1</v>
@@ -10632,7 +10966,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D152">
         <v>1</v>
@@ -10658,7 +10992,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D153">
         <v>1</v>
@@ -10690,7 +11024,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D154">
         <v>1</v>
@@ -10709,7 +11043,7 @@
         <v>154</v>
       </c>
       <c r="C155" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D155">
         <v>1</v>
@@ -10727,7 +11061,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D156">
         <v>1</v>
@@ -10747,7 +11081,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D157">
         <v>1</v>
@@ -10791,7 +11125,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D158">
         <v>1</v>
@@ -10813,7 +11147,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D159">
         <v>1</v>
@@ -10834,7 +11168,7 @@
         <v>159</v>
       </c>
       <c r="C160" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D160">
         <v>1</v>
@@ -10852,7 +11186,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D161">
         <v>1</v>
@@ -10905,7 +11239,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -10926,7 +11260,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D163">
         <v>1</v>
@@ -10947,7 +11281,7 @@
         <v>163</v>
       </c>
       <c r="C164" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -10965,7 +11299,7 @@
         <v>164</v>
       </c>
       <c r="C165" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D165">
         <v>1</v>
@@ -10983,7 +11317,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D166">
         <v>1</v>
@@ -11038,7 +11372,7 @@
         <v>166</v>
       </c>
       <c r="C167" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D167">
         <v>1</v>
@@ -11056,7 +11390,7 @@
         <v>167</v>
       </c>
       <c r="C168" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -11074,7 +11408,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D169">
         <v>1</v>
@@ -11130,7 +11464,7 @@
         <v>169</v>
       </c>
       <c r="C170" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D170">
         <v>1</v>
@@ -11148,7 +11482,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D171">
         <v>1</v>
@@ -11204,7 +11538,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D172">
         <v>1</v>
@@ -11266,7 +11600,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D173">
         <v>1</v>
@@ -11287,7 +11621,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>369</v>
+        <v>419</v>
       </c>
       <c r="D174">
         <v>1</v>
@@ -11308,17 +11642,13 @@
 final
 class
 FinalPersonClass {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 private
 final
 String name;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 private
 final
 int
 age;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 public
 FinalPersonClass(
 final
@@ -11326,32 +11656,24 @@
 final
 int
 age) {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 super
 ();
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 this
 .name = name;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 this
 .age = age;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; }
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+      }
 public
 int
 getAge() {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 return
 age;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; }
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+      }
 public
 String getName() {
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
 return
 name;
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; }
-&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+      }
 }',1);</v>
       </c>
     </row>
@@ -11363,7 +11685,7 @@
         <v>174</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D175">
         <v>1</v>
@@ -11382,7 +11704,7 @@
         <v>175</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D176">
         <v>1</v>
@@ -11402,7 +11724,7 @@
         <v>176</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D177">
         <v>1</v>
@@ -11424,7 +11746,7 @@
         <v>177</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D178">
         <v>1</v>
@@ -11442,7 +11764,7 @@
         <v>178</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D179">
         <v>1</v>
@@ -11466,7 +11788,7 @@
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D180">
         <v>1</v>
@@ -11501,7 +11823,7 @@
         <v>180</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D181">
         <v>1</v>
@@ -11526,7 +11848,7 @@
         <v>181</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D182">
         <v>1</v>
@@ -11546,7 +11868,7 @@
         <v>182</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -11567,7 +11889,7 @@
         <v>183</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D184">
         <v>1</v>
@@ -11591,7 +11913,7 @@
         <v>184</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D185">
         <v>1</v>
@@ -11619,7 +11941,7 @@
         <v>185</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D186">
         <v>1</v>
@@ -11661,7 +11983,7 @@
         <v>186</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D187">
         <v>1</v>
@@ -11703,7 +12025,7 @@
         <v>187</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D188">
         <v>1</v>
@@ -11732,7 +12054,7 @@
         <v>188</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D189">
         <v>1</v>
@@ -11754,7 +12076,7 @@
         <v>189</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -11772,7 +12094,7 @@
         <v>190</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -11841,7 +12163,7 @@
         <v>191</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D192">
         <v>1</v>
@@ -11886,7 +12208,7 @@
         <v>192</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D193">
         <v>1</v>
@@ -11907,7 +12229,7 @@
         <v>193</v>
       </c>
       <c r="C194" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D194">
         <v>1</v>
@@ -11925,7 +12247,7 @@
         <v>194</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D195">
         <v>1</v>
@@ -11952,7 +12274,7 @@
         <v>195</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D196">
         <v>1</v>
@@ -11975,7 +12297,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D197">
         <v>1</v>
@@ -11995,7 +12317,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D198">
         <v>1</v>
@@ -12017,7 +12339,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D199">
         <v>1</v>
@@ -12032,6 +12354,290 @@
 &lt;%@ page session="false"%&gt;',1);</v>
       </c>
     </row>
+    <row r="200" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200">
+        <v>199</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+      <c r="E200" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Answers values(199,199,'Ans) Java doesnt support multiple inheritance but it provide a way through which it can enact it. 
+Consider the scenario is C++
+Class A{
+public void add(){
+// some text
+}
+}
+Class B{
+public void add(){
+// some text
+}
+}
+Class C extends A,B{
+public static void main(String arg[]){
+C objC = new C();
+objC.add(); // problem, compiler gets confused and cant
+decide to call Class A or B method.
+}
+This problem is called Diamond problem.
+This problem in java is taken care with the use of interfaces
+In Java similar problem would look like:
+interface A{
+add();
+}
+interface B{
+add();
+}
+class C implements A,B{
+add(){
+// doesnt matter which interface it belong to
+}
+}',1);</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201">
+        <v>200</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
+      </c>
+      <c r="E201" t="str">
+        <f t="shared" ref="E201:E209" si="3">"insert into Answers values("&amp;A201&amp;","&amp;B201&amp;",'"&amp;C201&amp;"',"&amp;D201&amp;");"</f>
+        <v>insert into Answers values(200,200,'NO',1);</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202">
+        <v>201</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D202">
+        <v>1</v>
+      </c>
+      <c r="E202" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(201,201,'Ans) Java has a more expressive system of reference than most other garbage-collected programming languages, which allows for special behavior for garbage collection. A normal reference in Java is known as a strong reference. The java.lang.ref package defines three other types of references—soft, weak, and phantom references. Each type of reference is designed for a specific use.
+A SoftReference can be used to implement a cache. An object that is not reachable by a strong reference (that is, not strongly reachable), but is referenced by a soft reference is called softly reachable. A softly reachable object may be garbage collected at the discretion of the garbage collector. This generally means that softly reachable objects will only be garbage collected when free memory is low, but again, it is at the discretion of the garbage collector. Semantically, a soft reference means "keep this object unless the memory is needed."
+A WeakReference is used to implement weak maps. An object that is not strongly or softly reachable, but is referenced by a weak reference is called weakly reachable. A weakly reachable object will be garbage collected during the next collection cycle. This behavior is used in the class java.util.WeakHashMap. A weak map allows the programmer to put key/value pairs in the map and not worry about the objects taking up memory when the key is no longer reachable anywhere else. Another possible application of weak references is the string intern pool. Semantically, a weak reference means "get rid of this object when nothing else references it."
+A PhantomReference is used to reference objects that have been marked for garbage collection and have been finalized, but have not yet been reclaimed. An object that is not strongly, softly or weakly reachable, but is referenced by a phantom reference is called phantom reachable. This allows for more flexible cleanup than is possible with the finalization mechanism alone. Semantically, a phantom reference means "this object is no longer needed and has been finalized in preparation for being collected."',1);</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203">
+        <v>202</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+      <c r="E203" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(202,202,'Ans) The old generation''s default heap size can be overridden by using the -Xms and -Xmx switches to specify the initial and maximum sizes respectively: 
+java -Xms &lt;initial size&gt; -Xmx &lt;maximum size&gt; program
+For example: 
+java -Xms64m -Xmx128m program',1);</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204">
+        <v>203</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+      <c r="E204" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(203,203,'Ans) Differences are as follows:
+1) instanceof is a reserved word of Java, but isInstance(Object obj) is a method of java.lang.Class.
+if (obj instanceof MyType) {
+...
+}else if (MyType.class.isInstance(obj)) {
+...
+}
+2) instanceof is used of identify whether the object is type of a particular class or its subclass but isInstance(obj) is used to identify object of a particular class.',1);</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205">
+        <v>204</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+      <c r="E205" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(204,204,'Ans) Java supports only pass by value. The arguments passed as a parameter to a method is mainly primitive data types or objects. For the data type the actual value is passed.
+Java passes the references by value just like any other parameter. This means the references passed to the method are actually copies of the original references.Java copies and passes the reference by value, not the object. Thus, method manipulation will alter the objects, since the references point to the original objects.Consider the example:
+ public void tricky(Point arg1, Point arg2)
+ {
+   arg1.x = 100;
+   arg1.y = 100;
+   Point temp = arg1;
+   arg1 = arg2;
+   arg2 = temp;
+ }
+ public static void main(String [] args)
+ {
+   Point pnt1 = new Point(0,0);
+   Point pnt2 = new Point(0,0);
+   System.out.println("X: " + pnt1.x + " Y: " +pnt1.y); 
+   System.out.println("X: " + pnt2.x + " Y: " +pnt2.y);
+   System.out.println(" ");
+   tricky(pnt1,pnt2);
+   System.out.println("X: " + pnt1.x + " Y:" + pnt1.y); 
+   System.out.println("X: " + pnt2.x + " Y: " +pnt2.y); 
+ }
+OutPut:
+X: 0 Y: 0
+X: 0 Y: 0
+X: 100 Y: 100
+X: 0 Y: 0
+The method successfully alters the value of pnt1, even though it is passed by value; however, a swap of pnt1 and pnt2 fails! This is the major source of confusion. In the main() method, pnt1 and pnt2 are nothing more than object references. When you pass pnt1 and pnt2 to the tricky() method, Java passes the references by value just like any other parameter. This means the references passed to the method are actually copies of the original references.',1);</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206">
+        <v>205</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D206">
+        <v>1</v>
+      </c>
+      <c r="E206" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(205,205,'Ans) A memory leak is where an unreferenced object that will never be used again still hangs around in memory and doesnt get garbage collected.',1);</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207">
+        <v>206</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(206,206,'Ans) == operator is used to compare the references of the objects. 
+public bollean equals(Object o) is the method provided by the Object class. The default implementation uses == operator to compare two objects.
+But since the method can be overriden like for String class. equals() method can be used to compare the values of two objects.
+ String str1 = "MyName"; 
+ String str2 = "MyName";
+ String str3 = str2;
+ if(str1 == str2){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ if(str1.equals(str2)){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ Output:
+ Objects are not equal
+ Objects are equal
+ String str2 = "MyName";
+ String str3 = str2;
+ if(str2 == str3){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ if(str3.equals(str2)){
+ System.out.println("Objects are equal")
+ }else{
+ System.out.println("Objects are not equal")
+ }
+ OutPut:
+ Objects are equal
+ Objects are equal',1);</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208">
+        <v>207</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+      <c r="E208" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(207,207,'Ans) The @Override annotation can be added to the javadoc for the new method. If you accidently miss an argument or capitalize the method name wrong, the compiler will generate a compile-time error.',1);</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209">
+        <v>208</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D209">
+        <v>1</v>
+      </c>
+      <c r="E209" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into Answers values(208,208,'Ans)The heap size of an object can be found using -
+         Runtime.totalMemory()-Runtime.freeMemory() .',1);</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>